<commit_message>
halo_v2 JLCpcb files ready
</commit_message>
<xml_diff>
--- a/kicad_v2/gerber/halo-all-pos.xlsx
+++ b/kicad_v2/gerber/halo-all-pos.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="115">
   <si>
-    <t xml:space="preserve">Designator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mid X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mid Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation</t>
+    <t xml:space="preserve">Ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PosX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PosY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rot</t>
   </si>
   <si>
     <t xml:space="preserve">C1</t>
@@ -374,7 +374,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -407,6 +407,12 @@
       <name val="Open Sans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -460,12 +466,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -485,38 +491,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A107" activeCellId="0" sqref="A107"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="28.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="22.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="15.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" s="2" customFormat="true" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMH1" s="3"/>
+      <c r="AMI1" s="3"/>
+      <c r="AMJ1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -533,7 +540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -550,7 +557,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -567,7 +574,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -584,7 +591,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -601,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -618,24 +625,24 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>106.045</v>
+        <v>99.695</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>-73.025</v>
+        <v>-72.39</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -652,7 +659,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -669,7 +676,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -686,7 +693,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -703,7 +710,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -720,7 +727,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -737,7 +744,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -754,7 +761,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -771,12 +778,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>138.43</v>
+        <v>107.95</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>-114.3</v>
@@ -788,15 +795,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>143.51</v>
+        <v>149.86</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>-71.12</v>
+        <v>-79.4512</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>6</v>
@@ -805,7 +812,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -822,7 +829,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -839,7 +846,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -856,7 +863,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -873,7 +880,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -890,7 +897,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -907,7 +914,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -924,7 +931,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -941,7 +948,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -958,24 +965,24 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>62.23</v>
+        <v>60.96</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>-78.74</v>
+        <v>-72.39</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -992,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1009,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -1026,7 +1033,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -1043,7 +1050,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -1060,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -1077,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -1094,7 +1101,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -1111,7 +1118,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -1128,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1145,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1162,7 +1169,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1179,7 +1186,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -1196,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -1213,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -1230,7 +1237,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -1247,7 +1254,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -1264,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -1281,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -1298,7 +1305,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -1315,7 +1322,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -1332,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -1349,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -1366,7 +1373,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -1383,7 +1390,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -1400,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -1434,7 +1441,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -1451,7 +1458,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -1468,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
@@ -1485,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1502,7 +1509,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
@@ -1519,15 +1526,15 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>143.51</v>
+        <v>145.415</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>-80.01</v>
+        <v>-82.55</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>6</v>
@@ -1536,24 +1543,24 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>124.46</v>
+        <v>119.38</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>-80.01</v>
+        <v>-76.2</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="1" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -1570,7 +1577,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
@@ -1587,7 +1594,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
@@ -1604,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>70</v>
       </c>
@@ -1621,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>71</v>
       </c>
@@ -1638,7 +1645,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
@@ -1655,7 +1662,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>73</v>
       </c>
@@ -1672,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
@@ -1689,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>75</v>
       </c>
@@ -1706,7 +1713,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>76</v>
       </c>
@@ -1723,7 +1730,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>77</v>
       </c>
@@ -1740,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
@@ -1757,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>79</v>
       </c>
@@ -1774,7 +1781,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>80</v>
       </c>
@@ -1791,7 +1798,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>81</v>
       </c>
@@ -1808,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
@@ -1825,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
@@ -1842,7 +1849,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>84</v>
       </c>
@@ -1859,7 +1866,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -1876,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
@@ -1893,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -1910,7 +1917,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -1927,7 +1934,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>89</v>
       </c>
@@ -1944,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>90</v>
       </c>
@@ -1961,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>91</v>
       </c>
@@ -1978,7 +1985,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>92</v>
       </c>
@@ -1995,7 +2002,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>93</v>
       </c>
@@ -2012,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>94</v>
       </c>
@@ -2029,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>95</v>
       </c>
@@ -2046,7 +2053,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>96</v>
       </c>
@@ -2063,7 +2070,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>97</v>
       </c>
@@ -2080,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>98</v>
       </c>
@@ -2097,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>99</v>
       </c>
@@ -2114,7 +2121,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>100</v>
       </c>
@@ -2131,7 +2138,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>101</v>
       </c>
@@ -2148,7 +2155,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -2165,7 +2172,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
@@ -2182,7 +2189,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
@@ -2199,15 +2206,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B101" s="1" t="n">
-        <v>147.955</v>
+        <v>165.735</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>-71.12</v>
+        <v>-80.645</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>6</v>
@@ -2216,24 +2223,24 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B102" s="1" t="n">
-        <v>161.925</v>
+        <v>165.735</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>-71.12</v>
+        <v>-76.835</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E102" s="1" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
         <v>107</v>
       </c>
@@ -2250,7 +2257,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
         <v>108</v>
       </c>
@@ -2267,7 +2274,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
         <v>109</v>
       </c>
@@ -2284,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
@@ -2301,7 +2308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
         <v>111</v>
       </c>
@@ -2318,15 +2325,15 @@
         <v>180</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B108" s="1" t="n">
-        <v>190.589803</v>
+        <v>190.5</v>
       </c>
       <c r="C108" s="1" t="n">
-        <v>-78.829803</v>
+        <v>-78.74</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>6</v>
@@ -2335,7 +2342,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
@@ -2352,7 +2359,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
         <v>114</v>
       </c>
@@ -2369,7 +2376,6 @@
         <v>90</v>
       </c>
     </row>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>